<commit_message>
added test xls to be updated
</commit_message>
<xml_diff>
--- a/REFERENCES.xlsx
+++ b/REFERENCES.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="53">
   <si>
     <t>supplychainFundamentals</t>
   </si>
@@ -172,6 +172,9 @@
   </si>
   <si>
     <t>Credit channels for SMEs,non bank lending and supply chain finance history</t>
+  </si>
+  <si>
+    <t>https://www.investopedia.com/terms/s/supply-chain-finance.asp</t>
   </si>
 </sst>
 </file>
@@ -566,15 +569,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:C22"/>
+  <dimension ref="B2:C30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="C30" sqref="C30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="39" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="61.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="18" style="2" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -616,6 +619,11 @@
       </c>
       <c r="C22" s="2" t="s">
         <v>7</v>
+      </c>
+    </row>
+    <row r="30" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B30" s="1" t="s">
+        <v>52</v>
       </c>
     </row>
   </sheetData>
@@ -625,9 +633,10 @@
     <hyperlink ref="B21" r:id="rId3"/>
     <hyperlink ref="B22" r:id="rId4"/>
     <hyperlink ref="B4" r:id="rId5"/>
+    <hyperlink ref="B30" r:id="rId6"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId6"/>
+  <pageSetup orientation="portrait" r:id="rId7"/>
 </worksheet>
 </file>
 

</xml_diff>